<commit_message>
Commented out write statements
</commit_message>
<xml_diff>
--- a/3DQ5_MILESTONE_1_R7.xlsx
+++ b/3DQ5_MILESTONE_1_R7.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstje\Desktop\3DQ5_PROJECT\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8530E252-434F-4CD4-A642-D2270E1D3165}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="4410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="4410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,7 +522,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -954,7 +955,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{39615C8D-5386-401B-AAEE-86EAA7418A41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39615C8D-5386-401B-AAEE-86EAA7418A41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1023,7 +1024,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82025855-4A2A-4B23-9B1B-5B972497EB91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82025855-4A2A-4B23-9B1B-5B972497EB91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1088,7 +1089,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9CD07224-6C85-4AFC-A80F-3069ACC2E5C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CD07224-6C85-4AFC-A80F-3069ACC2E5C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1153,7 +1154,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{736BEF64-A133-4C2D-AD9B-7099E14EAD48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{736BEF64-A133-4C2D-AD9B-7099E14EAD48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,23 +1208,23 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>461010</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>474458</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>56254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>401782</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>20782</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>121024</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EA8B6B5-52C8-402A-BC8E-ED48E579F3FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA8B6B5-52C8-402A-BC8E-ED48E579F3FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1231,8 +1232,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12549101" y="447848"/>
-          <a:ext cx="5226281" cy="244879"/>
+          <a:off x="6906634" y="423807"/>
+          <a:ext cx="5252360" cy="248546"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1579,82 +1580,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BV50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO7" sqref="AO7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18" style="3" customWidth="1"/>
-    <col min="2" max="8" width="8.85546875" style="3"/>
-    <col min="9" max="9" width="8.85546875" style="10"/>
-    <col min="10" max="10" width="8.85546875" style="84" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="3"/>
-    <col min="12" max="12" width="8.85546875" style="10"/>
+    <col min="2" max="8" width="8.83984375" style="3"/>
+    <col min="9" max="9" width="8.83984375" style="10"/>
+    <col min="10" max="10" width="8.83984375" style="84" customWidth="1"/>
+    <col min="11" max="11" width="8.83984375" style="3"/>
+    <col min="12" max="12" width="8.83984375" style="10"/>
     <col min="13" max="13" width="12" style="84" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="101"/>
-    <col min="17" max="17" width="8.85546875" style="3"/>
-    <col min="18" max="18" width="11.42578125" style="10" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="84"/>
-    <col min="20" max="20" width="8.85546875" style="3"/>
-    <col min="21" max="21" width="8.85546875" style="10"/>
-    <col min="22" max="22" width="8.85546875" style="101" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="3"/>
-    <col min="24" max="24" width="8.85546875" style="10" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="84"/>
-    <col min="26" max="26" width="8.85546875" style="3"/>
-    <col min="27" max="27" width="8.85546875" style="10"/>
-    <col min="28" max="28" width="8.85546875" style="101"/>
-    <col min="29" max="29" width="8.85546875" style="3"/>
-    <col min="30" max="30" width="8.85546875" style="10"/>
-    <col min="31" max="31" width="8.85546875" style="84"/>
-    <col min="32" max="33" width="8.85546875" style="10"/>
-    <col min="34" max="34" width="8.85546875" style="101" customWidth="1"/>
-    <col min="35" max="35" width="8.85546875" style="19" customWidth="1"/>
-    <col min="36" max="36" width="8.85546875" style="26" customWidth="1"/>
-    <col min="37" max="37" width="8.85546875" style="84" customWidth="1"/>
-    <col min="38" max="38" width="8.85546875" style="50"/>
-    <col min="39" max="39" width="10.42578125" style="3" customWidth="1"/>
-    <col min="40" max="41" width="8.85546875" style="3"/>
-    <col min="42" max="42" width="11.42578125" style="3" customWidth="1"/>
-    <col min="43" max="43" width="8.85546875" style="3"/>
-    <col min="44" max="44" width="8.85546875" style="10"/>
-    <col min="45" max="45" width="12.42578125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="12.15625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="10.41796875" style="10" customWidth="1"/>
+    <col min="16" max="16" width="8.83984375" style="101"/>
+    <col min="17" max="17" width="8.83984375" style="3"/>
+    <col min="18" max="18" width="11.41796875" style="10" customWidth="1"/>
+    <col min="19" max="19" width="8.83984375" style="84"/>
+    <col min="20" max="20" width="8.83984375" style="3"/>
+    <col min="21" max="21" width="8.83984375" style="10"/>
+    <col min="22" max="22" width="8.83984375" style="101" customWidth="1"/>
+    <col min="23" max="23" width="8.83984375" style="3"/>
+    <col min="24" max="24" width="8.83984375" style="10" customWidth="1"/>
+    <col min="25" max="25" width="8.83984375" style="84"/>
+    <col min="26" max="26" width="8.83984375" style="3"/>
+    <col min="27" max="27" width="8.83984375" style="10"/>
+    <col min="28" max="28" width="8.83984375" style="101"/>
+    <col min="29" max="29" width="8.83984375" style="3"/>
+    <col min="30" max="30" width="8.83984375" style="10"/>
+    <col min="31" max="31" width="8.83984375" style="84"/>
+    <col min="32" max="33" width="8.83984375" style="10"/>
+    <col min="34" max="34" width="8.83984375" style="101" customWidth="1"/>
+    <col min="35" max="35" width="8.83984375" style="19" customWidth="1"/>
+    <col min="36" max="36" width="8.83984375" style="26" customWidth="1"/>
+    <col min="37" max="37" width="8.83984375" style="84" customWidth="1"/>
+    <col min="38" max="38" width="8.83984375" style="50"/>
+    <col min="39" max="39" width="10.41796875" style="3" customWidth="1"/>
+    <col min="40" max="41" width="8.83984375" style="3"/>
+    <col min="42" max="42" width="11.41796875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="8.83984375" style="3"/>
+    <col min="44" max="44" width="8.83984375" style="10"/>
+    <col min="45" max="45" width="12.41796875" style="10" customWidth="1"/>
     <col min="46" max="46" width="11" style="3" customWidth="1"/>
-    <col min="47" max="48" width="8.85546875" style="3"/>
-    <col min="49" max="49" width="13.5703125" style="3" customWidth="1"/>
-    <col min="50" max="50" width="8.85546875" style="3"/>
-    <col min="51" max="51" width="8.85546875" style="10"/>
-    <col min="52" max="52" width="14.42578125" style="10" customWidth="1"/>
+    <col min="47" max="48" width="8.83984375" style="3"/>
+    <col min="49" max="49" width="13.578125" style="3" customWidth="1"/>
+    <col min="50" max="50" width="8.83984375" style="3"/>
+    <col min="51" max="51" width="8.83984375" style="10"/>
+    <col min="52" max="52" width="14.41796875" style="10" customWidth="1"/>
     <col min="53" max="53" width="11" style="3" customWidth="1"/>
-    <col min="54" max="55" width="8.85546875" style="3"/>
-    <col min="56" max="56" width="13.5703125" style="3" customWidth="1"/>
-    <col min="57" max="57" width="8.85546875" style="3"/>
-    <col min="58" max="58" width="8.85546875" style="10"/>
-    <col min="59" max="59" width="14.42578125" style="10" customWidth="1"/>
+    <col min="54" max="55" width="8.83984375" style="3"/>
+    <col min="56" max="56" width="13.578125" style="3" customWidth="1"/>
+    <col min="57" max="57" width="8.83984375" style="3"/>
+    <col min="58" max="58" width="8.83984375" style="10"/>
+    <col min="59" max="59" width="14.41796875" style="10" customWidth="1"/>
     <col min="60" max="60" width="11" style="10" customWidth="1"/>
-    <col min="61" max="61" width="8.85546875" style="10"/>
-    <col min="62" max="62" width="8.85546875" style="3"/>
-    <col min="63" max="63" width="13.5703125" style="3" customWidth="1"/>
-    <col min="64" max="64" width="8.85546875" style="3"/>
-    <col min="65" max="65" width="8.85546875" style="10"/>
-    <col min="66" max="66" width="14.42578125" style="25" customWidth="1"/>
+    <col min="61" max="61" width="8.83984375" style="10"/>
+    <col min="62" max="62" width="8.83984375" style="3"/>
+    <col min="63" max="63" width="13.578125" style="3" customWidth="1"/>
+    <col min="64" max="64" width="8.83984375" style="3"/>
+    <col min="65" max="65" width="8.83984375" style="10"/>
+    <col min="66" max="66" width="14.41796875" style="25" customWidth="1"/>
     <col min="67" max="67" width="11" style="16" customWidth="1"/>
-    <col min="68" max="69" width="8.85546875" style="3"/>
-    <col min="70" max="70" width="13.5703125" style="3" customWidth="1"/>
-    <col min="71" max="71" width="8.85546875" style="3"/>
-    <col min="72" max="72" width="8.85546875" style="10"/>
-    <col min="73" max="73" width="8.85546875" style="25"/>
-    <col min="74" max="74" width="8.85546875" style="16"/>
-    <col min="75" max="16384" width="8.85546875" style="3"/>
+    <col min="68" max="69" width="8.83984375" style="3"/>
+    <col min="70" max="70" width="13.578125" style="3" customWidth="1"/>
+    <col min="71" max="71" width="8.83984375" style="3"/>
+    <col min="72" max="72" width="8.83984375" style="10"/>
+    <col min="73" max="73" width="8.83984375" style="25"/>
+    <col min="74" max="74" width="8.83984375" style="16"/>
+    <col min="75" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1781,7 @@
       <c r="BU1" s="70"/>
       <c r="BV1" s="13"/>
     </row>
-    <row r="2" spans="1:74" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1826,7 +1827,7 @@
       <c r="BU2" s="71"/>
       <c r="BV2" s="14"/>
     </row>
-    <row r="3" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1872,7 +1873,7 @@
       <c r="BU3" s="72"/>
       <c r="BV3" s="15"/>
     </row>
-    <row r="4" spans="1:74" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" s="112" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I4" s="113"/>
       <c r="J4" s="114"/>
       <c r="L4" s="113"/>
@@ -1912,7 +1913,7 @@
       <c r="BU4" s="118"/>
       <c r="BV4" s="119"/>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>139</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="43" t="s">
         <v>13</v>
       </c>
@@ -2162,7 +2163,7 @@
       <c r="BU7" s="62"/>
       <c r="BV7" s="46"/>
     </row>
-    <row r="9" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="43" t="s">
         <v>14</v>
       </c>
@@ -2236,7 +2237,7 @@
       <c r="BU9" s="62"/>
       <c r="BV9" s="46"/>
     </row>
-    <row r="10" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="43" t="s">
         <v>96</v>
       </c>
@@ -2296,7 +2297,7 @@
       <c r="BU10" s="62"/>
       <c r="BV10" s="46"/>
     </row>
-    <row r="11" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="43" t="s">
         <v>97</v>
       </c>
@@ -2352,7 +2353,7 @@
       <c r="BU11" s="62"/>
       <c r="BV11" s="46"/>
     </row>
-    <row r="12" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="43" t="s">
         <v>98</v>
       </c>
@@ -2410,7 +2411,7 @@
       <c r="BU12" s="62"/>
       <c r="BV12" s="46"/>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="L13" s="24"/>
       <c r="AM13" s="120"/>
       <c r="AN13" s="120"/>
@@ -2420,7 +2421,7 @@
       <c r="AR13" s="120"/>
       <c r="AS13" s="120"/>
     </row>
-    <row r="14" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="43" t="s">
         <v>65</v>
       </c>
@@ -2488,7 +2489,7 @@
       <c r="BU14" s="62"/>
       <c r="BV14" s="46"/>
     </row>
-    <row r="15" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:74" s="43" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="43" t="s">
         <v>66</v>
       </c>
@@ -2542,7 +2543,7 @@
       <c r="BU15" s="62"/>
       <c r="BV15" s="46"/>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="L17" s="24"/>
       <c r="AM17" s="120"/>
       <c r="AN17" s="120"/>
@@ -2552,7 +2553,7 @@
       <c r="AR17" s="120"/>
       <c r="AS17" s="120"/>
     </row>
-    <row r="18" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -2600,7 +2601,7 @@
       <c r="BU18" s="27"/>
       <c r="BV18" s="17"/>
     </row>
-    <row r="19" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="20" t="s">
         <v>5</v>
       </c>
@@ -2672,7 +2673,7 @@
       <c r="BU19" s="28"/>
       <c r="BV19" s="22"/>
     </row>
-    <row r="20" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="20" t="s">
         <v>6</v>
       </c>
@@ -2743,7 +2744,7 @@
       <c r="BU20" s="28"/>
       <c r="BV20" s="22"/>
     </row>
-    <row r="21" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="20" t="s">
         <v>7</v>
       </c>
@@ -2814,7 +2815,7 @@
       <c r="BU21" s="28"/>
       <c r="BV21" s="22"/>
     </row>
-    <row r="22" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="20" t="s">
         <v>8</v>
       </c>
@@ -2885,7 +2886,7 @@
       <c r="BU22" s="28"/>
       <c r="BV22" s="22"/>
     </row>
-    <row r="23" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="20" t="s">
         <v>9</v>
       </c>
@@ -2950,7 +2951,7 @@
       <c r="BU23" s="28"/>
       <c r="BV23" s="22"/>
     </row>
-    <row r="24" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="20" t="s">
         <v>10</v>
       </c>
@@ -3015,7 +3016,7 @@
       <c r="BU24" s="28"/>
       <c r="BV24" s="22"/>
     </row>
-    <row r="25" spans="1:74" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:74" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I25" s="12"/>
       <c r="J25" s="88"/>
       <c r="L25" s="12"/>
@@ -3060,7 +3061,7 @@
       <c r="BU25" s="29"/>
       <c r="BV25" s="18"/>
     </row>
-    <row r="28" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
@@ -3108,7 +3109,7 @@
       <c r="BU28" s="27"/>
       <c r="BV28" s="17"/>
     </row>
-    <row r="29" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20" t="s">
         <v>5</v>
       </c>
@@ -3178,7 +3179,7 @@
       <c r="BU29" s="28"/>
       <c r="BV29" s="22"/>
     </row>
-    <row r="30" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="20" t="s">
         <v>6</v>
       </c>
@@ -3248,7 +3249,7 @@
       <c r="BU30" s="28"/>
       <c r="BV30" s="22"/>
     </row>
-    <row r="31" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20" t="s">
         <v>7</v>
       </c>
@@ -3318,7 +3319,7 @@
       <c r="BU31" s="28"/>
       <c r="BV31" s="22"/>
     </row>
-    <row r="32" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
@@ -3388,7 +3389,7 @@
       <c r="BU32" s="28"/>
       <c r="BV32" s="22"/>
     </row>
-    <row r="33" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="20" t="s">
         <v>9</v>
       </c>
@@ -3452,7 +3453,7 @@
       <c r="BU33" s="28"/>
       <c r="BV33" s="22"/>
     </row>
-    <row r="34" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:74" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="20" t="s">
         <v>10</v>
       </c>
@@ -3516,7 +3517,7 @@
       <c r="BU34" s="28"/>
       <c r="BV34" s="22"/>
     </row>
-    <row r="35" spans="1:74" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:74" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I35" s="12"/>
       <c r="J35" s="88"/>
       <c r="L35" s="12"/>
@@ -3561,7 +3562,7 @@
       <c r="BU35" s="29"/>
       <c r="BV35" s="18"/>
     </row>
-    <row r="36" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I36" s="40"/>
       <c r="J36" s="89"/>
       <c r="L36" s="40"/>
@@ -3606,7 +3607,7 @@
       <c r="BU36" s="61"/>
       <c r="BV36" s="41"/>
     </row>
-    <row r="37" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I37" s="40"/>
       <c r="J37" s="89"/>
       <c r="L37" s="40"/>
@@ -3651,7 +3652,7 @@
       <c r="BU37" s="61"/>
       <c r="BV37" s="41"/>
     </row>
-    <row r="38" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="39" t="s">
         <v>41</v>
       </c>
@@ -3744,7 +3745,7 @@
       <c r="BU38" s="61"/>
       <c r="BV38" s="41"/>
     </row>
-    <row r="39" spans="1:74" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:74" s="47" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="47" t="s">
         <v>40</v>
       </c>
@@ -3813,7 +3814,7 @@
       <c r="BU39" s="73"/>
       <c r="BV39" s="58"/>
     </row>
-    <row r="40" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="39" t="s">
         <v>3</v>
       </c>
@@ -3934,7 +3935,7 @@
       <c r="BU40" s="61"/>
       <c r="BV40" s="41"/>
     </row>
-    <row r="42" spans="1:74" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:74" s="76" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="76" t="s">
         <v>57</v>
       </c>
@@ -3990,7 +3991,7 @@
       <c r="BU42" s="80"/>
       <c r="BV42" s="78"/>
     </row>
-    <row r="43" spans="1:74" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:74" s="76" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="76" t="s">
         <v>58</v>
       </c>
@@ -4048,7 +4049,7 @@
       <c r="BU43" s="80"/>
       <c r="BV43" s="78"/>
     </row>
-    <row r="46" spans="1:74" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:74" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="23" t="s">
         <v>26</v>
       </c>
@@ -4113,7 +4114,7 @@
       <c r="BU46" s="74"/>
       <c r="BV46" s="59"/>
     </row>
-    <row r="47" spans="1:74" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:74" s="30" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="30" t="s">
         <v>30</v>
       </c>
@@ -4176,7 +4177,7 @@
       <c r="BU47" s="75"/>
       <c r="BV47" s="60"/>
     </row>
-    <row r="48" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="39" t="s">
         <v>43</v>
       </c>
@@ -4286,7 +4287,7 @@
       <c r="BU48" s="61"/>
       <c r="BV48" s="41"/>
     </row>
-    <row r="50" spans="9:74" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:74" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I50" s="40"/>
       <c r="J50" s="89"/>
       <c r="L50" s="40"/>

</xml_diff>